<commit_message>
LoRa Configuration and Researching
</commit_message>
<xml_diff>
--- a/REFERENCES/Notes/schedular.xlsx
+++ b/REFERENCES/Notes/schedular.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HUST\Junior\2023-1\DATN\REFERENCES\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58A5D68-4F29-4F0D-8533-8F155BA468F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066D221C-36AC-4849-8B92-3BF71D44822C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{46F2DF86-DAAC-4A9F-ABC1-E2343732A84C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Tuần</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>21/09/2023</t>
+  </si>
+  <si>
+    <t>Setup truyền thông LoRa</t>
   </si>
 </sst>
 </file>
@@ -141,12 +144,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -462,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18B91C4-3578-4C39-9C97-51F5A9C3C56F}">
-  <dimension ref="A3:F9"/>
+  <dimension ref="A3:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -503,7 +512,7 @@
       <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -514,6 +523,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="36" x14ac:dyDescent="0.35">
+      <c r="B5" s="4"/>
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
@@ -522,6 +532,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="54" x14ac:dyDescent="0.35">
+      <c r="B6" s="4"/>
       <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
@@ -530,12 +541,13 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B7" s="4"/>
       <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -543,11 +555,22 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>2</v>
+      </c>
+      <c r="B10" s="5">
+        <v>44936</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>